<commit_message>
Update time sheet + quit function
</commit_message>
<xml_diff>
--- a/Project Inception/Time Sheet.xlsx
+++ b/Project Inception/Time Sheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>Michael</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Risk Register Organisational Risks</t>
   </si>
   <si>
+    <t>Total Time</t>
+  </si>
+  <si>
     <t>Project Plan</t>
   </si>
   <si>
@@ -55,31 +58,61 @@
     <t>Roles and responsibilities</t>
   </si>
   <si>
-    <t>Micheal</t>
-  </si>
-  <si>
     <t>Analysis of Alternatives, Proof reading and editing of PMP and Analysis of alternatives</t>
   </si>
   <si>
     <t>Risk Register,  Coding interface testing</t>
+  </si>
+  <si>
+    <t>Finalizing Risk Register and review on project plan</t>
+  </si>
+  <si>
+    <t>Studying the API</t>
+  </si>
+  <si>
+    <t>Learning the API</t>
+  </si>
+  <si>
+    <t>Clean up the code</t>
+  </si>
+  <si>
+    <t>Terminal menu</t>
+  </si>
+  <si>
+    <t>Setting backlogs</t>
+  </si>
+  <si>
+    <t>Studying the API (v2 and v3)</t>
+  </si>
+  <si>
+    <t>Playing around with the API (and incidentally creating initial code for downloading and plotting revisions)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Inconsolata"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,8 +149,20 @@
         <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border/>
     <border>
       <left style="thin">
@@ -129,6 +174,36 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -137,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -165,6 +240,9 @@
     <xf borderId="1" fillId="5" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -177,6 +255,10 @@
     <xf borderId="1" fillId="4" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -188,6 +270,60 @@
     </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="5" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="7" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="7" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
@@ -262,138 +398,398 @@
       <c r="D4" s="8">
         <v>43331.0</v>
       </c>
+      <c r="F4" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="9">
+      <c r="B5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="10">
         <v>0.6</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="11">
         <v>43334.0</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f>sumif(A4:A43,"*Michael*",C4:C43)</f>
+        <v>7.5</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="9">
+      <c r="B6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="10">
         <v>2.0</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="11">
         <v>43336.0</v>
       </c>
+      <c r="F6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f>sumif(A4:A43,"*Josh*",C4:C43)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="11">
+      <c r="B7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="12">
         <v>2.0</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="13">
         <v>43333.0</v>
       </c>
+      <c r="F7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="15">
+        <f>sumif(A4:A43,"*Keith*",C4:C43)</f>
+        <v>9.5</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="11">
+      <c r="B8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="12">
         <v>0.5</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="13">
         <v>43335.0</v>
       </c>
+      <c r="F8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <f>sumif(A4:A43,"*Simon*",C4:C43)</f>
+        <v>4.6</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="13" t="s">
+      <c r="A9" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="16">
         <v>3.5</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="17">
         <v>43336.0</v>
       </c>
+      <c r="F9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="15">
+        <f>sumif(A4:A43,"*Glyn*",C4:C43)</f>
+        <v>4.6</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="18">
         <v>3.0</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="19">
         <v>43335.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
+      <c r="A11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="D11" s="8">
+        <v>43336.0</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
+      <c r="A12" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="D12" s="17">
+        <v>43344.0</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
+      <c r="A13" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="D13" s="11">
+        <v>43345.0</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
+      <c r="A14" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="D14" s="20">
+        <v>43348.0</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
+      <c r="A15" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="18">
+        <v>1.0</v>
+      </c>
+      <c r="D15" s="21">
+        <v>43348.0</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
+      <c r="A16" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="D16" s="25">
+        <v>43345.0</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
+      <c r="A17" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="28">
+        <v>0.8</v>
+      </c>
+      <c r="D17" s="29">
+        <v>43348.0</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
+      <c r="A18" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="32">
+        <v>3.0</v>
+      </c>
+      <c r="D18" s="33">
+        <v>43344.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="36">
+        <v>4.0</v>
+      </c>
+      <c r="D19" s="37">
+        <v>43345.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="38"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="38"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="38"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="38"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="38"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="38"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="38"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="38"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="38"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="38"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="38"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="38"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="38"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="38"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="38"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="38"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="38"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="38"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="38"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="38"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="38"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="38"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>